<commit_message>
put pics instead of labels and buttons
</commit_message>
<xml_diff>
--- a/Physiotherapists.xlsx
+++ b/Physiotherapists.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yaels\יעל פרוייקט גמר\zedcheck\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E91491E-3803-421B-9AF1-3A9D75E9E9CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E35E9C17-03DE-4DAC-BFC5-61ED7FD67960}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -408,18 +408,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="9.75" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -429,9 +426,8 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>314808981</v>
       </c>
@@ -442,7 +438,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>12341234</v>
       </c>

</xml_diff>